<commit_message>
Working on 2022 data.
</commit_message>
<xml_diff>
--- a/data-raw/GHA-PSB.xlsx
+++ b/data-raw/GHA-PSB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1164A68-AD4F-3640-BAD9-51A5C01235A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D7D05B-A86F-3144-8743-F2805EF77031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
   <si>
     <t>Country</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>ktoe_to_TJ</t>
+  </si>
+  <si>
+    <t>TJ</t>
   </si>
 </sst>
 </file>
@@ -8119,7 +8122,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I2" sqref="I2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8224,7 +8227,7 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J2">
         <f>'FixedGHPSB ktoe original'!J2*Meta!$B$8</f>
@@ -8290,7 +8293,7 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J3">
         <f>'FixedGHPSB ktoe original'!J3*Meta!$B$8</f>
@@ -8356,7 +8359,7 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J4">
         <f>'FixedGHPSB ktoe original'!J4*Meta!$B$8</f>
@@ -8422,7 +8425,7 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J5">
         <f>'FixedGHPSB ktoe original'!J5*Meta!$B$8</f>
@@ -8488,7 +8491,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J6">
         <f>'FixedGHPSB ktoe original'!J6*Meta!$B$8</f>
@@ -8554,7 +8557,7 @@
         <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J7">
         <f>'FixedGHPSB ktoe original'!J7*Meta!$B$8</f>

</xml_diff>